<commit_message>
ENADID, Población con discapacidad en México
</commit_message>
<xml_diff>
--- a/Bases/ENADID_2023.xlsx
+++ b/Bases/ENADID_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github_Personal\Discapacidad_Mexico\Bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9101EB76-9203-496B-89F3-CE8354B3DCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C1932F-DF79-4A66-A085-94B37661845D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34452" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{054E0982-B31B-4B41-95B0-65AE04D970F8}"/>
+    <workbookView xWindow="34452" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{054E0982-B31B-4B41-95B0-65AE04D970F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Grupos de edad" sheetId="1" r:id="rId1"/>
@@ -494,9 +494,6 @@
     <t>El porcentaje se calculó con respecto al total de población de 15 años y más, para cada condición de discapacidad y sexo. Se excluye a la población que no especificó su edad.</t>
   </si>
   <si>
-    <t>Causas de la dificultad de la población de 5 años y más con discapacidad1¿, 2023</t>
-  </si>
-  <si>
     <t>El porcentaje se calcula con respecto al total de actividades con dificultad. Las opciones «Por su trabajo» y «Por uso de la tecnología» fueron creadas a partir de la codificación de las respuestas textuales registradas en la pregunta de causa de la dificultad</t>
   </si>
   <si>
@@ -531,6 +528,9 @@
   </si>
   <si>
     <t>Población de 5 años y más, por grupo quinquenal de edad y sexo, según condición de discapacidad</t>
+  </si>
+  <si>
+    <t>Causas de la dificultad de la población de 5 años y más con discapacidad, 2023</t>
   </si>
 </sst>
 </file>
@@ -1030,9 +1030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F12BDC-5492-4F6C-B140-EA6B918B28E2}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1042,7 +1040,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" x14ac:dyDescent="0.6">
       <c r="A1" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -1364,10 +1362,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="C23" s="34"/>
       <c r="D23" s="34"/>
@@ -1375,7 +1373,7 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="2"/>
       <c r="B24" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C24" s="34"/>
       <c r="D24" s="34"/>
@@ -1403,8 +1401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{268985DD-9E71-4C79-857E-DF484F9CAF7F}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:C37"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.45"/>
@@ -1416,12 +1414,12 @@
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -1800,7 +1798,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
@@ -1818,7 +1816,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.45"/>
@@ -1829,12 +1827,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -1968,7 +1966,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
@@ -1976,7 +1974,7 @@
         <v>128</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
@@ -1993,9 +1991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FAAE16-6D01-4151-AD8A-368702C859D1}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:B13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.45"/>
   <cols>
@@ -2005,7 +2001,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="32" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
@@ -2098,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
@@ -2106,7 +2102,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
@@ -2114,7 +2110,7 @@
         <v>128</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>